<commit_message>
Local search is hard to design
</commit_message>
<xml_diff>
--- a/info/soea/NBIPOPCMA-ES.xlsx
+++ b/info/soea/NBIPOPCMA-ES.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="D=10" sheetId="1" r:id="rId1"/>
@@ -13622,7 +13622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
@@ -14102,15 +14102,10 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
-      <c r="AC6" s="1">
-        <v>276.47058823529397</v>
-      </c>
+      <c r="AC6" s="1"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D7" s="1"/>
-      <c r="AC7">
-        <v>65.079137345596806</v>
-      </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
@@ -14227,6 +14222,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14234,7 +14230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>